<commit_message>
Added data scraping for weekly matchups. no longer have to manually harvest
</commit_message>
<xml_diff>
--- a/Predictions/Week 1/Week 1.xlsx
+++ b/Predictions/Week 1/Week 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg_yonan\Desktop\Tools\Programs\NFL\2025 Season\Predictions\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A55A52F-440A-4105-8957-2B17979A0368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC473630-8EDE-49DF-BB01-CE102551F746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed to relative paths. Added week 3 data
</commit_message>
<xml_diff>
--- a/Predictions/Week 1/Week 1.xlsx
+++ b/Predictions/Week 1/Week 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greg_yonan\Desktop\Tools\Programs\NFL\2025 Season\Predictions\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC473630-8EDE-49DF-BB01-CE102551F746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6D9B12-FC33-45BA-A235-75A2161ADC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,7 +157,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +204,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
         <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,6 +285,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,19 +659,19 @@
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -718,16 +728,16 @@
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -741,16 +751,16 @@
       <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -790,7 +800,7 @@
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="8" t="s">
@@ -879,16 +889,16 @@
       <c r="B13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -902,19 +912,19 @@
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="10" t="s">
         <v>31</v>
       </c>
     </row>
@@ -925,7 +935,7 @@
       <c r="B15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -934,7 +944,7 @@
       <c r="E15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -960,7 +970,7 @@
       <c r="F16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="10" t="s">
         <v>35</v>
       </c>
     </row>
@@ -983,8 +993,25 @@
       <c r="F17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G17" s="11" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.6875</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="G18" s="12">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>